<commit_message>
Come richiesto: nel test case avente id 47, aggiunto il valore mancante su colonna applicabilità. Tolto anche il valore "SI" nella colonna "TEST AUTOCERTIFICATO" della medesima riga.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GSQUAREDXX/Gsquared/ReSked/6.0/accreditamento-checklist_V8.2.7.xlsx
+++ b/GATEWAY/A1#111#GSQUAREDXX/Gsquared/ReSked/6.0/accreditamento-checklist_V8.2.7.xlsx
@@ -1931,7 +1931,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2036,12 +2036,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2250,7 +2244,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2419,10 +2413,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2435,7 +2425,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2826,7 +2816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="94" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="163.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -3966,11 +3956,11 @@
   <dimension ref="A1:W750"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="L10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="M30" activeCellId="0" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5067,11 +5057,13 @@
       <c r="G30" s="33"/>
       <c r="H30" s="33"/>
       <c r="I30" s="39"/>
-      <c r="J30" s="34"/>
+      <c r="J30" s="34" t="s">
+        <v>63</v>
+      </c>
       <c r="K30" s="34"/>
       <c r="L30" s="34"/>
       <c r="M30" s="34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N30" s="34" t="s">
         <v>63</v>
@@ -5092,9 +5084,7 @@
         <v>93</v>
       </c>
       <c r="T30" s="34"/>
-      <c r="U30" s="35" t="s">
-        <v>63</v>
-      </c>
+      <c r="U30" s="35"/>
       <c r="V30" s="36"/>
       <c r="W30" s="34" t="s">
         <v>54</v>
@@ -6040,7 +6030,7 @@
       <c r="E55" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="F55" s="42" t="n">
+      <c r="F55" s="33" t="n">
         <v>46048</v>
       </c>
       <c r="G55" s="39" t="s">
@@ -11037,7 +11027,7 @@
       <c r="B186" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C186" s="43" t="s">
+      <c r="C186" s="42" t="s">
         <v>59</v>
       </c>
       <c r="D186" s="30" t="s">
@@ -11322,7 +11312,7 @@
       <c r="D193" s="30" t="s">
         <v>447</v>
       </c>
-      <c r="E193" s="44" t="s">
+      <c r="E193" s="43" t="s">
         <v>448</v>
       </c>
       <c r="F193" s="33"/>
@@ -15434,7 +15424,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>452</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -15446,158 +15436,158 @@
       <c r="D1" s="19" t="s">
         <v>454</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="45" t="s">
         <v>455</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="46" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>458</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="49" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="48" t="s">
         <v>460</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="49" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="48" t="s">
         <v>462</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="50" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="48" t="s">
         <v>464</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="49" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="48" t="s">
         <v>466</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="48" t="s">
         <v>468</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="50" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="48" t="s">
         <v>470</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="50" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="48" t="s">
         <v>472</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="50" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="36.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="47" t="s">
         <v>474</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="51" t="s">
         <v>475</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="49" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>457</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="48" t="s">
         <v>477</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="50" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D12" s="53"/>
+      <c r="D12" s="52"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D13" s="53"/>
+      <c r="D13" s="52"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -16578,32 +16568,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="53" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>479</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="53" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>480</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Corretto test case 25 (id 471).
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GSQUAREDXX/Gsquared/ReSked/6.0/accreditamento-checklist_V8.2.7.xlsx
+++ b/GATEWAY/A1#111#GSQUAREDXX/Gsquared/ReSked/6.0/accreditamento-checklist_V8.2.7.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
@@ -859,9 +859,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">Campo/sezione non gestito/a in modo strutturato dall’applicativo</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT18_KO</t>
   </si>
   <si>
@@ -1760,13 +1757,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-01-26T10:21:21.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">372e1ad0b25c2356a87b298a1f69b8f1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.455854493f20645227e7f443fbe39f13a1c1df094693d43eb7944bc7f8ddbe18.7b14ea6fa9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-03T13:14:21.000000Z </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2772734ea5eef1593aa69a94d0254af8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.04b54ed75d7aa0a3bf6374dafe854e35641c6e5c2e6a72fc00ef0f196a7d67e8.28d18f1a99^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT26</t>
@@ -1827,6 +1824,9 @@
   </si>
   <si>
     <t xml:space="preserve">Razionale di Applicabilità</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campo/sezione non gestito/a in modo strutturato dall’applicativo</t>
   </si>
   <si>
     <t xml:space="preserve">Campo valorizzato di default</t>
@@ -3956,11 +3956,11 @@
   <dimension ref="A1:W750"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="L10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E68" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M30" activeCellId="0" sqref="M30"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
+      <selection pane="bottomRight" activeCell="K68" activeCellId="0" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3969,7 +3969,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="63.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="104.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="74.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="1" width="33.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="27.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="11" style="1" width="36.45"/>
@@ -6384,7 +6384,7 @@
         <v>65</v>
       </c>
       <c r="K62" s="34" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="L62" s="34"/>
       <c r="M62" s="34"/>
@@ -6412,10 +6412,10 @@
         <v>59</v>
       </c>
       <c r="D63" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E63" s="31" t="s">
         <v>173</v>
-      </c>
-      <c r="E63" s="31" t="s">
-        <v>174</v>
       </c>
       <c r="F63" s="33"/>
       <c r="G63" s="33"/>
@@ -6425,7 +6425,7 @@
         <v>65</v>
       </c>
       <c r="K63" s="34" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="L63" s="34"/>
       <c r="M63" s="34"/>
@@ -6453,10 +6453,10 @@
         <v>59</v>
       </c>
       <c r="D64" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" s="31" t="s">
         <v>175</v>
-      </c>
-      <c r="E64" s="31" t="s">
-        <v>176</v>
       </c>
       <c r="F64" s="33"/>
       <c r="G64" s="33"/>
@@ -6466,7 +6466,7 @@
         <v>65</v>
       </c>
       <c r="K64" s="34" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="L64" s="34"/>
       <c r="M64" s="34"/>
@@ -6494,10 +6494,10 @@
         <v>59</v>
       </c>
       <c r="D65" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" s="31" t="s">
         <v>177</v>
-      </c>
-      <c r="E65" s="31" t="s">
-        <v>178</v>
       </c>
       <c r="F65" s="33"/>
       <c r="G65" s="33"/>
@@ -6507,7 +6507,7 @@
         <v>65</v>
       </c>
       <c r="K65" s="34" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="L65" s="34"/>
       <c r="M65" s="34"/>
@@ -6535,10 +6535,10 @@
         <v>59</v>
       </c>
       <c r="D66" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="E66" s="31" t="s">
         <v>179</v>
-      </c>
-      <c r="E66" s="31" t="s">
-        <v>180</v>
       </c>
       <c r="F66" s="33"/>
       <c r="G66" s="33"/>
@@ -6548,7 +6548,7 @@
         <v>65</v>
       </c>
       <c r="K66" s="34" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="L66" s="34"/>
       <c r="M66" s="34"/>
@@ -6576,22 +6576,22 @@
         <v>59</v>
       </c>
       <c r="D67" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="E67" s="31" t="s">
         <v>181</v>
-      </c>
-      <c r="E67" s="31" t="s">
-        <v>182</v>
       </c>
       <c r="F67" s="33" t="n">
         <v>46048</v>
       </c>
       <c r="G67" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="H67" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="H67" s="39" t="s">
+      <c r="I67" s="39" t="s">
         <v>184</v>
-      </c>
-      <c r="I67" s="39" t="s">
-        <v>185</v>
       </c>
       <c r="J67" s="34" t="s">
         <v>63</v>
@@ -6605,7 +6605,7 @@
         <v>63</v>
       </c>
       <c r="O67" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P67" s="34" t="s">
         <v>63</v>
@@ -6617,7 +6617,7 @@
         <v>63</v>
       </c>
       <c r="S67" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T67" s="34"/>
       <c r="U67" s="35"/>
@@ -6637,10 +6637,10 @@
         <v>59</v>
       </c>
       <c r="D68" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="E68" s="31" t="s">
         <v>188</v>
-      </c>
-      <c r="E68" s="31" t="s">
-        <v>189</v>
       </c>
       <c r="F68" s="33"/>
       <c r="G68" s="33"/>
@@ -6650,7 +6650,7 @@
         <v>65</v>
       </c>
       <c r="K68" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L68" s="34"/>
       <c r="M68" s="34"/>
@@ -6678,10 +6678,10 @@
         <v>69</v>
       </c>
       <c r="D69" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="E69" s="31" t="s">
         <v>191</v>
-      </c>
-      <c r="E69" s="31" t="s">
-        <v>192</v>
       </c>
       <c r="F69" s="33"/>
       <c r="G69" s="33"/>
@@ -6715,10 +6715,10 @@
         <v>69</v>
       </c>
       <c r="D70" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="E70" s="31" t="s">
         <v>193</v>
-      </c>
-      <c r="E70" s="31" t="s">
-        <v>194</v>
       </c>
       <c r="F70" s="33"/>
       <c r="G70" s="33"/>
@@ -6752,10 +6752,10 @@
         <v>69</v>
       </c>
       <c r="D71" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E71" s="31" t="s">
         <v>195</v>
-      </c>
-      <c r="E71" s="31" t="s">
-        <v>196</v>
       </c>
       <c r="F71" s="33"/>
       <c r="G71" s="33"/>
@@ -6789,10 +6789,10 @@
         <v>69</v>
       </c>
       <c r="D72" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="E72" s="31" t="s">
         <v>197</v>
-      </c>
-      <c r="E72" s="31" t="s">
-        <v>198</v>
       </c>
       <c r="F72" s="33"/>
       <c r="G72" s="33"/>
@@ -6826,10 +6826,10 @@
         <v>69</v>
       </c>
       <c r="D73" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="E73" s="31" t="s">
         <v>199</v>
-      </c>
-      <c r="E73" s="31" t="s">
-        <v>200</v>
       </c>
       <c r="F73" s="33"/>
       <c r="G73" s="33"/>
@@ -6863,10 +6863,10 @@
         <v>69</v>
       </c>
       <c r="D74" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="E74" s="31" t="s">
         <v>201</v>
-      </c>
-      <c r="E74" s="31" t="s">
-        <v>202</v>
       </c>
       <c r="F74" s="33"/>
       <c r="G74" s="33"/>
@@ -6900,10 +6900,10 @@
         <v>69</v>
       </c>
       <c r="D75" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="E75" s="31" t="s">
         <v>203</v>
-      </c>
-      <c r="E75" s="31" t="s">
-        <v>204</v>
       </c>
       <c r="F75" s="33"/>
       <c r="G75" s="33"/>
@@ -6937,10 +6937,10 @@
         <v>69</v>
       </c>
       <c r="D76" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="E76" s="31" t="s">
         <v>205</v>
-      </c>
-      <c r="E76" s="31" t="s">
-        <v>206</v>
       </c>
       <c r="F76" s="33"/>
       <c r="G76" s="33"/>
@@ -6974,10 +6974,10 @@
         <v>69</v>
       </c>
       <c r="D77" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="E77" s="31" t="s">
         <v>207</v>
-      </c>
-      <c r="E77" s="31" t="s">
-        <v>208</v>
       </c>
       <c r="F77" s="33"/>
       <c r="G77" s="33"/>
@@ -7011,10 +7011,10 @@
         <v>69</v>
       </c>
       <c r="D78" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="E78" s="31" t="s">
         <v>209</v>
-      </c>
-      <c r="E78" s="31" t="s">
-        <v>210</v>
       </c>
       <c r="F78" s="33"/>
       <c r="G78" s="33"/>
@@ -7048,10 +7048,10 @@
         <v>69</v>
       </c>
       <c r="D79" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E79" s="31" t="s">
         <v>211</v>
-      </c>
-      <c r="E79" s="31" t="s">
-        <v>212</v>
       </c>
       <c r="F79" s="33"/>
       <c r="G79" s="33"/>
@@ -7085,10 +7085,10 @@
         <v>71</v>
       </c>
       <c r="D80" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="E80" s="31" t="s">
         <v>213</v>
-      </c>
-      <c r="E80" s="31" t="s">
-        <v>214</v>
       </c>
       <c r="F80" s="33"/>
       <c r="G80" s="33"/>
@@ -7122,10 +7122,10 @@
         <v>71</v>
       </c>
       <c r="D81" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="E81" s="31" t="s">
         <v>215</v>
-      </c>
-      <c r="E81" s="31" t="s">
-        <v>216</v>
       </c>
       <c r="F81" s="33"/>
       <c r="G81" s="33"/>
@@ -7159,10 +7159,10 @@
         <v>71</v>
       </c>
       <c r="D82" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="E82" s="31" t="s">
         <v>217</v>
-      </c>
-      <c r="E82" s="31" t="s">
-        <v>218</v>
       </c>
       <c r="F82" s="33"/>
       <c r="G82" s="33"/>
@@ -7196,10 +7196,10 @@
         <v>71</v>
       </c>
       <c r="D83" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="E83" s="31" t="s">
         <v>219</v>
-      </c>
-      <c r="E83" s="31" t="s">
-        <v>220</v>
       </c>
       <c r="F83" s="33"/>
       <c r="G83" s="33"/>
@@ -7233,10 +7233,10 @@
         <v>71</v>
       </c>
       <c r="D84" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="E84" s="31" t="s">
         <v>221</v>
-      </c>
-      <c r="E84" s="31" t="s">
-        <v>222</v>
       </c>
       <c r="F84" s="33"/>
       <c r="G84" s="33"/>
@@ -7270,10 +7270,10 @@
         <v>71</v>
       </c>
       <c r="D85" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="E85" s="31" t="s">
         <v>223</v>
-      </c>
-      <c r="E85" s="31" t="s">
-        <v>224</v>
       </c>
       <c r="F85" s="33"/>
       <c r="G85" s="33"/>
@@ -7307,10 +7307,10 @@
         <v>71</v>
       </c>
       <c r="D86" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="E86" s="31" t="s">
         <v>225</v>
-      </c>
-      <c r="E86" s="31" t="s">
-        <v>226</v>
       </c>
       <c r="F86" s="33"/>
       <c r="G86" s="33"/>
@@ -7344,10 +7344,10 @@
         <v>71</v>
       </c>
       <c r="D87" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="E87" s="31" t="s">
         <v>227</v>
-      </c>
-      <c r="E87" s="31" t="s">
-        <v>228</v>
       </c>
       <c r="F87" s="33"/>
       <c r="G87" s="33"/>
@@ -7381,10 +7381,10 @@
         <v>71</v>
       </c>
       <c r="D88" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="E88" s="31" t="s">
         <v>229</v>
-      </c>
-      <c r="E88" s="31" t="s">
-        <v>230</v>
       </c>
       <c r="F88" s="33"/>
       <c r="G88" s="33"/>
@@ -7418,10 +7418,10 @@
         <v>71</v>
       </c>
       <c r="D89" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="E89" s="31" t="s">
         <v>231</v>
-      </c>
-      <c r="E89" s="31" t="s">
-        <v>232</v>
       </c>
       <c r="F89" s="33"/>
       <c r="G89" s="33"/>
@@ -7455,10 +7455,10 @@
         <v>71</v>
       </c>
       <c r="D90" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E90" s="31" t="s">
         <v>233</v>
-      </c>
-      <c r="E90" s="31" t="s">
-        <v>234</v>
       </c>
       <c r="F90" s="33"/>
       <c r="G90" s="33"/>
@@ -7492,10 +7492,10 @@
         <v>71</v>
       </c>
       <c r="D91" s="30" t="s">
+        <v>234</v>
+      </c>
+      <c r="E91" s="31" t="s">
         <v>235</v>
-      </c>
-      <c r="E91" s="31" t="s">
-        <v>236</v>
       </c>
       <c r="F91" s="33"/>
       <c r="G91" s="33"/>
@@ -7529,10 +7529,10 @@
         <v>71</v>
       </c>
       <c r="D92" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="E92" s="31" t="s">
         <v>237</v>
-      </c>
-      <c r="E92" s="31" t="s">
-        <v>238</v>
       </c>
       <c r="F92" s="33"/>
       <c r="G92" s="33"/>
@@ -7566,10 +7566,10 @@
         <v>73</v>
       </c>
       <c r="D93" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="E93" s="31" t="s">
         <v>239</v>
-      </c>
-      <c r="E93" s="31" t="s">
-        <v>240</v>
       </c>
       <c r="F93" s="33"/>
       <c r="G93" s="33"/>
@@ -7603,10 +7603,10 @@
         <v>73</v>
       </c>
       <c r="D94" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="E94" s="31" t="s">
         <v>241</v>
-      </c>
-      <c r="E94" s="31" t="s">
-        <v>242</v>
       </c>
       <c r="F94" s="33"/>
       <c r="G94" s="33"/>
@@ -7640,10 +7640,10 @@
         <v>73</v>
       </c>
       <c r="D95" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="E95" s="31" t="s">
         <v>243</v>
-      </c>
-      <c r="E95" s="31" t="s">
-        <v>244</v>
       </c>
       <c r="F95" s="33"/>
       <c r="G95" s="33"/>
@@ -7677,10 +7677,10 @@
         <v>73</v>
       </c>
       <c r="D96" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="E96" s="31" t="s">
         <v>245</v>
-      </c>
-      <c r="E96" s="31" t="s">
-        <v>246</v>
       </c>
       <c r="F96" s="33"/>
       <c r="G96" s="33"/>
@@ -7714,10 +7714,10 @@
         <v>73</v>
       </c>
       <c r="D97" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E97" s="31" t="s">
         <v>247</v>
-      </c>
-      <c r="E97" s="31" t="s">
-        <v>248</v>
       </c>
       <c r="F97" s="33"/>
       <c r="G97" s="33"/>
@@ -7751,10 +7751,10 @@
         <v>73</v>
       </c>
       <c r="D98" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="E98" s="31" t="s">
         <v>249</v>
-      </c>
-      <c r="E98" s="31" t="s">
-        <v>250</v>
       </c>
       <c r="F98" s="33"/>
       <c r="G98" s="33"/>
@@ -7788,10 +7788,10 @@
         <v>73</v>
       </c>
       <c r="D99" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="E99" s="31" t="s">
         <v>251</v>
-      </c>
-      <c r="E99" s="31" t="s">
-        <v>252</v>
       </c>
       <c r="F99" s="33"/>
       <c r="G99" s="33"/>
@@ -7825,10 +7825,10 @@
         <v>73</v>
       </c>
       <c r="D100" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="E100" s="31" t="s">
         <v>253</v>
-      </c>
-      <c r="E100" s="31" t="s">
-        <v>254</v>
       </c>
       <c r="F100" s="33"/>
       <c r="G100" s="33"/>
@@ -7862,10 +7862,10 @@
         <v>73</v>
       </c>
       <c r="D101" s="30" t="s">
+        <v>254</v>
+      </c>
+      <c r="E101" s="31" t="s">
         <v>255</v>
-      </c>
-      <c r="E101" s="31" t="s">
-        <v>256</v>
       </c>
       <c r="F101" s="33"/>
       <c r="G101" s="33"/>
@@ -7899,10 +7899,10 @@
         <v>73</v>
       </c>
       <c r="D102" s="30" t="s">
+        <v>256</v>
+      </c>
+      <c r="E102" s="31" t="s">
         <v>257</v>
-      </c>
-      <c r="E102" s="31" t="s">
-        <v>258</v>
       </c>
       <c r="F102" s="33"/>
       <c r="G102" s="33"/>
@@ -7936,10 +7936,10 @@
         <v>73</v>
       </c>
       <c r="D103" s="30" t="s">
+        <v>258</v>
+      </c>
+      <c r="E103" s="31" t="s">
         <v>259</v>
-      </c>
-      <c r="E103" s="31" t="s">
-        <v>260</v>
       </c>
       <c r="F103" s="33"/>
       <c r="G103" s="33"/>
@@ -7973,10 +7973,10 @@
         <v>73</v>
       </c>
       <c r="D104" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="E104" s="31" t="s">
         <v>261</v>
-      </c>
-      <c r="E104" s="31" t="s">
-        <v>262</v>
       </c>
       <c r="F104" s="33"/>
       <c r="G104" s="33"/>
@@ -8010,10 +8010,10 @@
         <v>73</v>
       </c>
       <c r="D105" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="E105" s="31" t="s">
         <v>263</v>
-      </c>
-      <c r="E105" s="31" t="s">
-        <v>264</v>
       </c>
       <c r="F105" s="33"/>
       <c r="G105" s="33"/>
@@ -8047,10 +8047,10 @@
         <v>73</v>
       </c>
       <c r="D106" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="E106" s="31" t="s">
         <v>265</v>
-      </c>
-      <c r="E106" s="31" t="s">
-        <v>266</v>
       </c>
       <c r="F106" s="33"/>
       <c r="G106" s="33"/>
@@ -8084,10 +8084,10 @@
         <v>73</v>
       </c>
       <c r="D107" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="E107" s="31" t="s">
         <v>267</v>
-      </c>
-      <c r="E107" s="31" t="s">
-        <v>268</v>
       </c>
       <c r="F107" s="33"/>
       <c r="G107" s="33"/>
@@ -8121,10 +8121,10 @@
         <v>73</v>
       </c>
       <c r="D108" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="E108" s="31" t="s">
         <v>269</v>
-      </c>
-      <c r="E108" s="31" t="s">
-        <v>270</v>
       </c>
       <c r="F108" s="33"/>
       <c r="G108" s="33"/>
@@ -8158,10 +8158,10 @@
         <v>73</v>
       </c>
       <c r="D109" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="E109" s="31" t="s">
         <v>271</v>
-      </c>
-      <c r="E109" s="31" t="s">
-        <v>272</v>
       </c>
       <c r="F109" s="33"/>
       <c r="G109" s="33"/>
@@ -8195,10 +8195,10 @@
         <v>73</v>
       </c>
       <c r="D110" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="E110" s="31" t="s">
         <v>273</v>
-      </c>
-      <c r="E110" s="31" t="s">
-        <v>274</v>
       </c>
       <c r="F110" s="33"/>
       <c r="G110" s="33"/>
@@ -8232,10 +8232,10 @@
         <v>73</v>
       </c>
       <c r="D111" s="30" t="s">
+        <v>274</v>
+      </c>
+      <c r="E111" s="31" t="s">
         <v>275</v>
-      </c>
-      <c r="E111" s="31" t="s">
-        <v>276</v>
       </c>
       <c r="F111" s="33"/>
       <c r="G111" s="33"/>
@@ -8269,10 +8269,10 @@
         <v>73</v>
       </c>
       <c r="D112" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="E112" s="31" t="s">
         <v>277</v>
-      </c>
-      <c r="E112" s="31" t="s">
-        <v>278</v>
       </c>
       <c r="F112" s="33"/>
       <c r="G112" s="33"/>
@@ -8306,10 +8306,10 @@
         <v>73</v>
       </c>
       <c r="D113" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="E113" s="31" t="s">
         <v>279</v>
-      </c>
-      <c r="E113" s="31" t="s">
-        <v>280</v>
       </c>
       <c r="F113" s="33"/>
       <c r="G113" s="33"/>
@@ -8343,10 +8343,10 @@
         <v>73</v>
       </c>
       <c r="D114" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="E114" s="31" t="s">
         <v>281</v>
-      </c>
-      <c r="E114" s="31" t="s">
-        <v>282</v>
       </c>
       <c r="F114" s="33"/>
       <c r="G114" s="33"/>
@@ -8380,10 +8380,10 @@
         <v>73</v>
       </c>
       <c r="D115" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="E115" s="31" t="s">
         <v>283</v>
-      </c>
-      <c r="E115" s="31" t="s">
-        <v>284</v>
       </c>
       <c r="F115" s="33"/>
       <c r="G115" s="33"/>
@@ -8417,10 +8417,10 @@
         <v>67</v>
       </c>
       <c r="D116" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="E116" s="31" t="s">
         <v>285</v>
-      </c>
-      <c r="E116" s="31" t="s">
-        <v>286</v>
       </c>
       <c r="F116" s="33"/>
       <c r="G116" s="33"/>
@@ -8454,10 +8454,10 @@
         <v>67</v>
       </c>
       <c r="D117" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="E117" s="31" t="s">
         <v>287</v>
-      </c>
-      <c r="E117" s="31" t="s">
-        <v>288</v>
       </c>
       <c r="F117" s="33"/>
       <c r="G117" s="33"/>
@@ -8491,10 +8491,10 @@
         <v>67</v>
       </c>
       <c r="D118" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E118" s="31" t="s">
         <v>289</v>
-      </c>
-      <c r="E118" s="31" t="s">
-        <v>290</v>
       </c>
       <c r="F118" s="33"/>
       <c r="G118" s="33"/>
@@ -8528,10 +8528,10 @@
         <v>67</v>
       </c>
       <c r="D119" s="30" t="s">
+        <v>290</v>
+      </c>
+      <c r="E119" s="31" t="s">
         <v>291</v>
-      </c>
-      <c r="E119" s="31" t="s">
-        <v>292</v>
       </c>
       <c r="F119" s="33"/>
       <c r="G119" s="33"/>
@@ -8565,10 +8565,10 @@
         <v>67</v>
       </c>
       <c r="D120" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="E120" s="31" t="s">
         <v>293</v>
-      </c>
-      <c r="E120" s="31" t="s">
-        <v>294</v>
       </c>
       <c r="F120" s="33"/>
       <c r="G120" s="33"/>
@@ -8602,10 +8602,10 @@
         <v>67</v>
       </c>
       <c r="D121" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="E121" s="31" t="s">
         <v>295</v>
-      </c>
-      <c r="E121" s="31" t="s">
-        <v>296</v>
       </c>
       <c r="F121" s="33"/>
       <c r="G121" s="33"/>
@@ -8639,10 +8639,10 @@
         <v>67</v>
       </c>
       <c r="D122" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="E122" s="31" t="s">
         <v>297</v>
-      </c>
-      <c r="E122" s="31" t="s">
-        <v>298</v>
       </c>
       <c r="F122" s="33"/>
       <c r="G122" s="33"/>
@@ -8676,10 +8676,10 @@
         <v>67</v>
       </c>
       <c r="D123" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="E123" s="31" t="s">
         <v>299</v>
-      </c>
-      <c r="E123" s="31" t="s">
-        <v>300</v>
       </c>
       <c r="F123" s="33"/>
       <c r="G123" s="33"/>
@@ -8713,10 +8713,10 @@
         <v>67</v>
       </c>
       <c r="D124" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="E124" s="31" t="s">
         <v>301</v>
-      </c>
-      <c r="E124" s="31" t="s">
-        <v>302</v>
       </c>
       <c r="F124" s="33"/>
       <c r="G124" s="33"/>
@@ -8750,10 +8750,10 @@
         <v>67</v>
       </c>
       <c r="D125" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="E125" s="31" t="s">
         <v>303</v>
-      </c>
-      <c r="E125" s="31" t="s">
-        <v>304</v>
       </c>
       <c r="F125" s="33"/>
       <c r="G125" s="33"/>
@@ -8787,10 +8787,10 @@
         <v>67</v>
       </c>
       <c r="D126" s="30" t="s">
+        <v>304</v>
+      </c>
+      <c r="E126" s="31" t="s">
         <v>305</v>
-      </c>
-      <c r="E126" s="31" t="s">
-        <v>306</v>
       </c>
       <c r="F126" s="33"/>
       <c r="G126" s="33"/>
@@ -8824,10 +8824,10 @@
         <v>67</v>
       </c>
       <c r="D127" s="30" t="s">
+        <v>306</v>
+      </c>
+      <c r="E127" s="31" t="s">
         <v>307</v>
-      </c>
-      <c r="E127" s="31" t="s">
-        <v>308</v>
       </c>
       <c r="F127" s="33"/>
       <c r="G127" s="33"/>
@@ -8861,10 +8861,10 @@
         <v>67</v>
       </c>
       <c r="D128" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="E128" s="31" t="s">
         <v>309</v>
-      </c>
-      <c r="E128" s="31" t="s">
-        <v>310</v>
       </c>
       <c r="F128" s="33"/>
       <c r="G128" s="33"/>
@@ -8898,10 +8898,10 @@
         <v>67</v>
       </c>
       <c r="D129" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="E129" s="31" t="s">
         <v>311</v>
-      </c>
-      <c r="E129" s="31" t="s">
-        <v>312</v>
       </c>
       <c r="F129" s="33"/>
       <c r="G129" s="33"/>
@@ -8935,10 +8935,10 @@
         <v>67</v>
       </c>
       <c r="D130" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="E130" s="31" t="s">
         <v>313</v>
-      </c>
-      <c r="E130" s="31" t="s">
-        <v>314</v>
       </c>
       <c r="F130" s="33"/>
       <c r="G130" s="33"/>
@@ -8972,10 +8972,10 @@
         <v>57</v>
       </c>
       <c r="D131" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="E131" s="31" t="s">
         <v>315</v>
-      </c>
-      <c r="E131" s="31" t="s">
-        <v>316</v>
       </c>
       <c r="F131" s="33"/>
       <c r="G131" s="33"/>
@@ -9009,10 +9009,10 @@
         <v>57</v>
       </c>
       <c r="D132" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="E132" s="31" t="s">
         <v>317</v>
-      </c>
-      <c r="E132" s="31" t="s">
-        <v>318</v>
       </c>
       <c r="F132" s="33"/>
       <c r="G132" s="33"/>
@@ -9046,10 +9046,10 @@
         <v>57</v>
       </c>
       <c r="D133" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="E133" s="31" t="s">
         <v>319</v>
-      </c>
-      <c r="E133" s="31" t="s">
-        <v>320</v>
       </c>
       <c r="F133" s="33"/>
       <c r="G133" s="33"/>
@@ -9083,10 +9083,10 @@
         <v>57</v>
       </c>
       <c r="D134" s="30" t="s">
+        <v>320</v>
+      </c>
+      <c r="E134" s="31" t="s">
         <v>321</v>
-      </c>
-      <c r="E134" s="31" t="s">
-        <v>322</v>
       </c>
       <c r="F134" s="33"/>
       <c r="G134" s="33"/>
@@ -9120,10 +9120,10 @@
         <v>57</v>
       </c>
       <c r="D135" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="E135" s="31" t="s">
         <v>323</v>
-      </c>
-      <c r="E135" s="31" t="s">
-        <v>324</v>
       </c>
       <c r="F135" s="33"/>
       <c r="G135" s="33"/>
@@ -9157,10 +9157,10 @@
         <v>57</v>
       </c>
       <c r="D136" s="30" t="s">
+        <v>324</v>
+      </c>
+      <c r="E136" s="31" t="s">
         <v>325</v>
-      </c>
-      <c r="E136" s="31" t="s">
-        <v>326</v>
       </c>
       <c r="F136" s="33"/>
       <c r="G136" s="33"/>
@@ -9194,10 +9194,10 @@
         <v>57</v>
       </c>
       <c r="D137" s="30" t="s">
+        <v>326</v>
+      </c>
+      <c r="E137" s="31" t="s">
         <v>327</v>
-      </c>
-      <c r="E137" s="31" t="s">
-        <v>328</v>
       </c>
       <c r="F137" s="33"/>
       <c r="G137" s="33"/>
@@ -9231,10 +9231,10 @@
         <v>57</v>
       </c>
       <c r="D138" s="30" t="s">
+        <v>328</v>
+      </c>
+      <c r="E138" s="31" t="s">
         <v>329</v>
-      </c>
-      <c r="E138" s="31" t="s">
-        <v>330</v>
       </c>
       <c r="F138" s="33"/>
       <c r="G138" s="33"/>
@@ -9268,10 +9268,10 @@
         <v>57</v>
       </c>
       <c r="D139" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="E139" s="31" t="s">
         <v>331</v>
-      </c>
-      <c r="E139" s="31" t="s">
-        <v>332</v>
       </c>
       <c r="F139" s="33"/>
       <c r="G139" s="33"/>
@@ -9305,10 +9305,10 @@
         <v>57</v>
       </c>
       <c r="D140" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="E140" s="31" t="s">
         <v>333</v>
-      </c>
-      <c r="E140" s="31" t="s">
-        <v>334</v>
       </c>
       <c r="F140" s="33"/>
       <c r="G140" s="33"/>
@@ -9342,10 +9342,10 @@
         <v>57</v>
       </c>
       <c r="D141" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="E141" s="31" t="s">
         <v>335</v>
-      </c>
-      <c r="E141" s="31" t="s">
-        <v>336</v>
       </c>
       <c r="F141" s="33"/>
       <c r="G141" s="33"/>
@@ -9379,10 +9379,10 @@
         <v>57</v>
       </c>
       <c r="D142" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="E142" s="31" t="s">
         <v>337</v>
-      </c>
-      <c r="E142" s="31" t="s">
-        <v>338</v>
       </c>
       <c r="F142" s="33"/>
       <c r="G142" s="33"/>
@@ -9416,10 +9416,10 @@
         <v>57</v>
       </c>
       <c r="D143" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="E143" s="31" t="s">
         <v>339</v>
-      </c>
-      <c r="E143" s="31" t="s">
-        <v>340</v>
       </c>
       <c r="F143" s="33"/>
       <c r="G143" s="33"/>
@@ -9453,10 +9453,10 @@
         <v>57</v>
       </c>
       <c r="D144" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="E144" s="31" t="s">
         <v>341</v>
-      </c>
-      <c r="E144" s="31" t="s">
-        <v>342</v>
       </c>
       <c r="F144" s="33"/>
       <c r="G144" s="33"/>
@@ -9490,10 +9490,10 @@
         <v>57</v>
       </c>
       <c r="D145" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="E145" s="31" t="s">
         <v>343</v>
-      </c>
-      <c r="E145" s="31" t="s">
-        <v>344</v>
       </c>
       <c r="F145" s="33"/>
       <c r="G145" s="33"/>
@@ -9527,10 +9527,10 @@
         <v>48</v>
       </c>
       <c r="D146" s="30" t="s">
+        <v>344</v>
+      </c>
+      <c r="E146" s="31" t="s">
         <v>345</v>
-      </c>
-      <c r="E146" s="31" t="s">
-        <v>346</v>
       </c>
       <c r="F146" s="33"/>
       <c r="G146" s="33"/>
@@ -9564,10 +9564,10 @@
         <v>48</v>
       </c>
       <c r="D147" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="E147" s="31" t="s">
         <v>347</v>
-      </c>
-      <c r="E147" s="31" t="s">
-        <v>348</v>
       </c>
       <c r="F147" s="33"/>
       <c r="G147" s="33"/>
@@ -9598,13 +9598,13 @@
         <v>47</v>
       </c>
       <c r="C148" s="37" t="s">
+        <v>348</v>
+      </c>
+      <c r="D148" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="D148" s="30" t="s">
+      <c r="E148" s="31" t="s">
         <v>350</v>
-      </c>
-      <c r="E148" s="31" t="s">
-        <v>351</v>
       </c>
       <c r="F148" s="33"/>
       <c r="G148" s="33"/>
@@ -9635,13 +9635,13 @@
         <v>47</v>
       </c>
       <c r="C149" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D149" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="E149" s="31" t="s">
         <v>352</v>
-      </c>
-      <c r="E149" s="31" t="s">
-        <v>353</v>
       </c>
       <c r="F149" s="33"/>
       <c r="G149" s="33"/>
@@ -9672,13 +9672,13 @@
         <v>47</v>
       </c>
       <c r="C150" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D150" s="30" t="s">
+        <v>353</v>
+      </c>
+      <c r="E150" s="31" t="s">
         <v>354</v>
-      </c>
-      <c r="E150" s="31" t="s">
-        <v>355</v>
       </c>
       <c r="F150" s="33"/>
       <c r="G150" s="33"/>
@@ -9709,10 +9709,10 @@
         <v>47</v>
       </c>
       <c r="C151" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D151" s="30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E151" s="38" t="s">
         <v>53</v>
@@ -9746,10 +9746,10 @@
         <v>47</v>
       </c>
       <c r="C152" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D152" s="30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E152" s="38" t="s">
         <v>76</v>
@@ -9783,13 +9783,13 @@
         <v>47</v>
       </c>
       <c r="C153" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D153" s="30" t="s">
+        <v>357</v>
+      </c>
+      <c r="E153" s="31" t="s">
         <v>358</v>
-      </c>
-      <c r="E153" s="31" t="s">
-        <v>359</v>
       </c>
       <c r="F153" s="33"/>
       <c r="G153" s="33"/>
@@ -9820,13 +9820,13 @@
         <v>47</v>
       </c>
       <c r="C154" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D154" s="30" t="s">
+        <v>359</v>
+      </c>
+      <c r="E154" s="31" t="s">
         <v>360</v>
-      </c>
-      <c r="E154" s="31" t="s">
-        <v>361</v>
       </c>
       <c r="F154" s="33"/>
       <c r="G154" s="33"/>
@@ -9857,13 +9857,13 @@
         <v>47</v>
       </c>
       <c r="C155" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D155" s="30" t="s">
+        <v>361</v>
+      </c>
+      <c r="E155" s="31" t="s">
         <v>362</v>
-      </c>
-      <c r="E155" s="31" t="s">
-        <v>363</v>
       </c>
       <c r="F155" s="33"/>
       <c r="G155" s="33"/>
@@ -9894,13 +9894,13 @@
         <v>47</v>
       </c>
       <c r="C156" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D156" s="30" t="s">
+        <v>363</v>
+      </c>
+      <c r="E156" s="31" t="s">
         <v>364</v>
-      </c>
-      <c r="E156" s="31" t="s">
-        <v>365</v>
       </c>
       <c r="F156" s="33"/>
       <c r="G156" s="33"/>
@@ -9931,13 +9931,13 @@
         <v>47</v>
       </c>
       <c r="C157" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D157" s="30" t="s">
+        <v>365</v>
+      </c>
+      <c r="E157" s="31" t="s">
         <v>366</v>
-      </c>
-      <c r="E157" s="31" t="s">
-        <v>367</v>
       </c>
       <c r="F157" s="33"/>
       <c r="G157" s="33"/>
@@ -9968,13 +9968,13 @@
         <v>47</v>
       </c>
       <c r="C158" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D158" s="30" t="s">
+        <v>367</v>
+      </c>
+      <c r="E158" s="31" t="s">
         <v>368</v>
-      </c>
-      <c r="E158" s="31" t="s">
-        <v>369</v>
       </c>
       <c r="F158" s="33"/>
       <c r="G158" s="33"/>
@@ -10005,13 +10005,13 @@
         <v>47</v>
       </c>
       <c r="C159" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D159" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="E159" s="31" t="s">
         <v>370</v>
-      </c>
-      <c r="E159" s="31" t="s">
-        <v>371</v>
       </c>
       <c r="F159" s="33"/>
       <c r="G159" s="33"/>
@@ -10042,13 +10042,13 @@
         <v>47</v>
       </c>
       <c r="C160" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D160" s="30" t="s">
+        <v>371</v>
+      </c>
+      <c r="E160" s="31" t="s">
         <v>372</v>
-      </c>
-      <c r="E160" s="31" t="s">
-        <v>373</v>
       </c>
       <c r="F160" s="33"/>
       <c r="G160" s="33"/>
@@ -10079,13 +10079,13 @@
         <v>47</v>
       </c>
       <c r="C161" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D161" s="30" t="s">
+        <v>373</v>
+      </c>
+      <c r="E161" s="31" t="s">
         <v>374</v>
-      </c>
-      <c r="E161" s="31" t="s">
-        <v>375</v>
       </c>
       <c r="F161" s="33"/>
       <c r="G161" s="33"/>
@@ -10116,13 +10116,13 @@
         <v>47</v>
       </c>
       <c r="C162" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D162" s="30" t="s">
+        <v>375</v>
+      </c>
+      <c r="E162" s="31" t="s">
         <v>376</v>
-      </c>
-      <c r="E162" s="31" t="s">
-        <v>377</v>
       </c>
       <c r="F162" s="33"/>
       <c r="G162" s="33"/>
@@ -10153,13 +10153,13 @@
         <v>47</v>
       </c>
       <c r="C163" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D163" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="E163" s="31" t="s">
         <v>378</v>
-      </c>
-      <c r="E163" s="31" t="s">
-        <v>379</v>
       </c>
       <c r="F163" s="33"/>
       <c r="G163" s="33"/>
@@ -10193,10 +10193,10 @@
         <v>67</v>
       </c>
       <c r="D164" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="E164" s="31" t="s">
         <v>380</v>
-      </c>
-      <c r="E164" s="31" t="s">
-        <v>381</v>
       </c>
       <c r="F164" s="33"/>
       <c r="G164" s="33"/>
@@ -10230,10 +10230,10 @@
         <v>67</v>
       </c>
       <c r="D165" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="E165" s="31" t="s">
         <v>382</v>
-      </c>
-      <c r="E165" s="31" t="s">
-        <v>383</v>
       </c>
       <c r="F165" s="33"/>
       <c r="G165" s="33"/>
@@ -10267,10 +10267,10 @@
         <v>55</v>
       </c>
       <c r="D166" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="E166" s="31" t="s">
         <v>384</v>
-      </c>
-      <c r="E166" s="31" t="s">
-        <v>385</v>
       </c>
       <c r="F166" s="33"/>
       <c r="G166" s="33"/>
@@ -10304,10 +10304,10 @@
         <v>55</v>
       </c>
       <c r="D167" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="E167" s="31" t="s">
         <v>386</v>
-      </c>
-      <c r="E167" s="31" t="s">
-        <v>387</v>
       </c>
       <c r="F167" s="33"/>
       <c r="G167" s="33"/>
@@ -10341,10 +10341,10 @@
         <v>48</v>
       </c>
       <c r="D168" s="30" t="s">
+        <v>387</v>
+      </c>
+      <c r="E168" s="31" t="s">
         <v>388</v>
-      </c>
-      <c r="E168" s="31" t="s">
-        <v>389</v>
       </c>
       <c r="F168" s="33"/>
       <c r="G168" s="33"/>
@@ -10378,10 +10378,10 @@
         <v>73</v>
       </c>
       <c r="D169" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="E169" s="31" t="s">
         <v>390</v>
-      </c>
-      <c r="E169" s="31" t="s">
-        <v>391</v>
       </c>
       <c r="F169" s="33"/>
       <c r="G169" s="33"/>
@@ -10415,10 +10415,10 @@
         <v>73</v>
       </c>
       <c r="D170" s="30" t="s">
+        <v>391</v>
+      </c>
+      <c r="E170" s="31" t="s">
         <v>392</v>
-      </c>
-      <c r="E170" s="31" t="s">
-        <v>393</v>
       </c>
       <c r="F170" s="33"/>
       <c r="G170" s="33"/>
@@ -10452,10 +10452,10 @@
         <v>71</v>
       </c>
       <c r="D171" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="E171" s="31" t="s">
         <v>394</v>
-      </c>
-      <c r="E171" s="31" t="s">
-        <v>395</v>
       </c>
       <c r="F171" s="33"/>
       <c r="G171" s="33"/>
@@ -10489,10 +10489,10 @@
         <v>71</v>
       </c>
       <c r="D172" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="E172" s="31" t="s">
         <v>396</v>
-      </c>
-      <c r="E172" s="31" t="s">
-        <v>397</v>
       </c>
       <c r="F172" s="33"/>
       <c r="G172" s="33"/>
@@ -10526,10 +10526,10 @@
         <v>69</v>
       </c>
       <c r="D173" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="E173" s="31" t="s">
         <v>398</v>
-      </c>
-      <c r="E173" s="31" t="s">
-        <v>399</v>
       </c>
       <c r="F173" s="33"/>
       <c r="G173" s="33"/>
@@ -10563,10 +10563,10 @@
         <v>69</v>
       </c>
       <c r="D174" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="E174" s="31" t="s">
         <v>400</v>
-      </c>
-      <c r="E174" s="31" t="s">
-        <v>401</v>
       </c>
       <c r="F174" s="33"/>
       <c r="G174" s="33"/>
@@ -10597,13 +10597,13 @@
         <v>47</v>
       </c>
       <c r="C175" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D175" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="E175" s="31" t="s">
         <v>402</v>
-      </c>
-      <c r="E175" s="31" t="s">
-        <v>403</v>
       </c>
       <c r="F175" s="33"/>
       <c r="G175" s="33"/>
@@ -10637,10 +10637,10 @@
         <v>67</v>
       </c>
       <c r="D176" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="E176" s="31" t="s">
         <v>404</v>
-      </c>
-      <c r="E176" s="31" t="s">
-        <v>405</v>
       </c>
       <c r="F176" s="30"/>
       <c r="G176" s="30"/>
@@ -10674,22 +10674,22 @@
         <v>59</v>
       </c>
       <c r="D177" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="E177" s="31" t="s">
         <v>406</v>
-      </c>
-      <c r="E177" s="31" t="s">
-        <v>407</v>
       </c>
       <c r="F177" s="33" t="n">
         <v>46048</v>
       </c>
       <c r="G177" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="H177" s="33" t="s">
         <v>408</v>
       </c>
-      <c r="H177" s="33" t="s">
+      <c r="I177" s="39" t="s">
         <v>409</v>
-      </c>
-      <c r="I177" s="39" t="s">
-        <v>410</v>
       </c>
       <c r="J177" s="34" t="s">
         <v>63</v>
@@ -10703,7 +10703,7 @@
         <v>63</v>
       </c>
       <c r="O177" s="34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="P177" s="34" t="s">
         <v>63</v>
@@ -10715,7 +10715,7 @@
         <v>63</v>
       </c>
       <c r="S177" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T177" s="34"/>
       <c r="U177" s="30"/>
@@ -10735,10 +10735,10 @@
         <v>73</v>
       </c>
       <c r="D178" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="E178" s="31" t="s">
         <v>412</v>
-      </c>
-      <c r="E178" s="31" t="s">
-        <v>413</v>
       </c>
       <c r="F178" s="30"/>
       <c r="G178" s="30"/>
@@ -10772,10 +10772,10 @@
         <v>69</v>
       </c>
       <c r="D179" s="30" t="s">
+        <v>413</v>
+      </c>
+      <c r="E179" s="31" t="s">
         <v>414</v>
-      </c>
-      <c r="E179" s="31" t="s">
-        <v>415</v>
       </c>
       <c r="F179" s="30"/>
       <c r="G179" s="30"/>
@@ -10809,10 +10809,10 @@
         <v>71</v>
       </c>
       <c r="D180" s="30" t="s">
+        <v>415</v>
+      </c>
+      <c r="E180" s="31" t="s">
         <v>416</v>
-      </c>
-      <c r="E180" s="31" t="s">
-        <v>417</v>
       </c>
       <c r="F180" s="30"/>
       <c r="G180" s="30"/>
@@ -10846,10 +10846,10 @@
         <v>48</v>
       </c>
       <c r="D181" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="E181" s="31" t="s">
         <v>418</v>
-      </c>
-      <c r="E181" s="31" t="s">
-        <v>419</v>
       </c>
       <c r="F181" s="30"/>
       <c r="G181" s="30"/>
@@ -10883,10 +10883,10 @@
         <v>55</v>
       </c>
       <c r="D182" s="30" t="s">
+        <v>419</v>
+      </c>
+      <c r="E182" s="31" t="s">
         <v>420</v>
-      </c>
-      <c r="E182" s="31" t="s">
-        <v>421</v>
       </c>
       <c r="F182" s="30"/>
       <c r="G182" s="30"/>
@@ -10920,10 +10920,10 @@
         <v>67</v>
       </c>
       <c r="D183" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="E183" s="31" t="s">
         <v>422</v>
-      </c>
-      <c r="E183" s="31" t="s">
-        <v>423</v>
       </c>
       <c r="F183" s="30"/>
       <c r="G183" s="30"/>
@@ -10957,10 +10957,10 @@
         <v>57</v>
       </c>
       <c r="D184" s="30" t="s">
+        <v>423</v>
+      </c>
+      <c r="E184" s="31" t="s">
         <v>424</v>
-      </c>
-      <c r="E184" s="31" t="s">
-        <v>425</v>
       </c>
       <c r="F184" s="30"/>
       <c r="G184" s="30"/>
@@ -10991,13 +10991,13 @@
         <v>47</v>
       </c>
       <c r="C185" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D185" s="30" t="s">
+        <v>425</v>
+      </c>
+      <c r="E185" s="31" t="s">
         <v>426</v>
-      </c>
-      <c r="E185" s="31" t="s">
-        <v>427</v>
       </c>
       <c r="F185" s="30"/>
       <c r="G185" s="30"/>
@@ -11031,22 +11031,22 @@
         <v>59</v>
       </c>
       <c r="D186" s="30" t="s">
+        <v>427</v>
+      </c>
+      <c r="E186" s="31" t="s">
         <v>428</v>
-      </c>
-      <c r="E186" s="31" t="s">
-        <v>429</v>
       </c>
       <c r="F186" s="39" t="n">
         <v>46048</v>
       </c>
-      <c r="G186" s="39" t="s">
+      <c r="G186" s="33" t="s">
+        <v>429</v>
+      </c>
+      <c r="H186" s="34" t="s">
         <v>430</v>
       </c>
-      <c r="H186" s="39" t="s">
+      <c r="I186" s="34" t="s">
         <v>431</v>
-      </c>
-      <c r="I186" s="39" t="s">
-        <v>432</v>
       </c>
       <c r="J186" s="34" t="s">
         <v>63</v>
@@ -11078,10 +11078,10 @@
         <v>59</v>
       </c>
       <c r="D187" s="30" t="s">
+        <v>432</v>
+      </c>
+      <c r="E187" s="31" t="s">
         <v>433</v>
-      </c>
-      <c r="E187" s="31" t="s">
-        <v>434</v>
       </c>
       <c r="F187" s="33"/>
       <c r="G187" s="33"/>
@@ -11091,10 +11091,10 @@
         <v>65</v>
       </c>
       <c r="K187" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="L187" s="34" t="s">
         <v>435</v>
-      </c>
-      <c r="L187" s="34" t="s">
-        <v>436</v>
       </c>
       <c r="M187" s="34"/>
       <c r="N187" s="34"/>
@@ -11121,10 +11121,10 @@
         <v>48</v>
       </c>
       <c r="D188" s="37" t="s">
+        <v>436</v>
+      </c>
+      <c r="E188" s="31" t="s">
         <v>437</v>
-      </c>
-      <c r="E188" s="31" t="s">
-        <v>438</v>
       </c>
       <c r="F188" s="33"/>
       <c r="G188" s="33"/>
@@ -11158,10 +11158,10 @@
         <v>59</v>
       </c>
       <c r="D189" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="E189" s="31" t="s">
         <v>439</v>
-      </c>
-      <c r="E189" s="31" t="s">
-        <v>440</v>
       </c>
       <c r="F189" s="33"/>
       <c r="G189" s="33"/>
@@ -11171,7 +11171,7 @@
         <v>65</v>
       </c>
       <c r="K189" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L189" s="34"/>
       <c r="M189" s="34"/>
@@ -11199,10 +11199,10 @@
         <v>67</v>
       </c>
       <c r="D190" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="E190" s="31" t="s">
         <v>441</v>
-      </c>
-      <c r="E190" s="31" t="s">
-        <v>442</v>
       </c>
       <c r="F190" s="33"/>
       <c r="G190" s="33"/>
@@ -11236,10 +11236,10 @@
         <v>57</v>
       </c>
       <c r="D191" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="E191" s="31" t="s">
         <v>443</v>
-      </c>
-      <c r="E191" s="31" t="s">
-        <v>444</v>
       </c>
       <c r="F191" s="33"/>
       <c r="G191" s="33"/>
@@ -11273,10 +11273,10 @@
         <v>57</v>
       </c>
       <c r="D192" s="30" t="s">
+        <v>444</v>
+      </c>
+      <c r="E192" s="31" t="s">
         <v>445</v>
-      </c>
-      <c r="E192" s="31" t="s">
-        <v>446</v>
       </c>
       <c r="F192" s="33"/>
       <c r="G192" s="33"/>
@@ -11310,10 +11310,10 @@
         <v>57</v>
       </c>
       <c r="D193" s="30" t="s">
+        <v>446</v>
+      </c>
+      <c r="E193" s="43" t="s">
         <v>447</v>
-      </c>
-      <c r="E193" s="43" t="s">
-        <v>448</v>
       </c>
       <c r="F193" s="33"/>
       <c r="G193" s="33"/>
@@ -15310,7 +15310,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J10:J193 M10:N55 P10:R21 O22:R22 P23:R55 M56:O56 Q56:R56 M57:N193 P57:R193" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J10:J187 M10:N55 P10:R21 O22:R22 P23:R55 M56:O56 Q56:R56 M57:N193 P57:R193 H186:I186 J188:J193" type="list">
       <formula1>Sheet1!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -15350,12 +15350,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>172</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15375,7 +15375,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15385,7 +15385,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -15571,7 +15571,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="47" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>457</v>

</xml_diff>

<commit_message>
Corretti errori su intervalli date mancanti.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GSQUAREDXX/Gsquared/ReSked/6.0/accreditamento-checklist_V8.2.7.xlsx
+++ b/GATEWAY/A1#111#GSQUAREDXX/Gsquared/ReSked/6.0/accreditamento-checklist_V8.2.7.xlsx
@@ -1757,13 +1757,13 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-03T13:14:21.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2772734ea5eef1593aa69a94d0254af8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.04b54ed75d7aa0a3bf6374dafe854e35641c6e5c2e6a72fc00ef0f196a7d67e8.28d18f1a99^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-05T16:45:16.000000Z </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6a2637346a46f3eed9087b2337ad9f64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.068903c591f88636d4e4d57ea4e5ebdd2ca921580ea8de264d7ced19993d71d1.845540672a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RAD_CT26</t>
@@ -3960,7 +3960,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
-      <selection pane="bottomRight" activeCell="K68" activeCellId="0" sqref="K68"/>
+      <selection pane="bottomRight" activeCell="I187" activeCellId="0" sqref="I187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11037,15 +11037,15 @@
         <v>428</v>
       </c>
       <c r="F186" s="39" t="n">
-        <v>46048</v>
+        <v>46058</v>
       </c>
       <c r="G186" s="33" t="s">
         <v>429</v>
       </c>
-      <c r="H186" s="34" t="s">
+      <c r="H186" s="33" t="s">
         <v>430</v>
       </c>
-      <c r="I186" s="34" t="s">
+      <c r="I186" s="39" t="s">
         <v>431</v>
       </c>
       <c r="J186" s="34" t="s">
@@ -15310,7 +15310,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J10:J187 M10:N55 P10:R21 O22:R22 P23:R55 M56:O56 Q56:R56 M57:N193 P57:R193 H186:I186 J188:J193" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J10:J193 M10:N55 P10:R21 O22:R22 P23:R55 M56:O56 Q56:R56 M57:N193 P57:R193" type="list">
       <formula1>Sheet1!$B$2:$B$3</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Effettuati nuovi test: - sistemato problema date antecedenti l'ultimo test accreditato - sistemato problema test 448
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GSQUAREDXX/Gsquared/ReSked/6.0/accreditamento-checklist_V8.2.7.xlsx
+++ b/GATEWAY/A1#111#GSQUAREDXX/Gsquared/ReSked/6.0/accreditamento-checklist_V8.2.7.xlsx
@@ -475,10 +475,10 @@
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_RSA_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-09T11:10:13.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">b9eb222b5a9280b7d2ef2d0df6a705c1 </t>
+    <t xml:space="preserve">2026-02-24T14:26:44.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a58b25dbe68edb3b294b9c1224358424</t>
   </si>
   <si>
     <t xml:space="preserve">CERT_VAC</t>
@@ -573,10 +573,10 @@
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_RSA_KO</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-09T11:10:26.000000Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f72aee7118cf9b389673da6a15773aad </t>
+    <t xml:space="preserve">2026-02-24T14:33:19.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2b67e91fd7098aeb32106981f5d326c9</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_CERT_VAC_KO</t>
@@ -1274,13 +1274,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-10T09:16:22.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1d6c6a0c66a91d3d4bc22a421e186d99 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.f5dad03ce9eb274cf3cbe4a017c5a605f51e5fbe6fec209b3f280cd921a865e7.6dadef043f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2026-02-24T14:37:10.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25c40af7a5072865adc4fe03c777b31d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.165d6671706f68e70e524470472a0efd9aee4e5495d9acf59f8fdf0ddd6c1efc.46e2754320^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ] </t>
@@ -1293,13 +1293,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-10T09:57:32.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9ada14bca7a708bd45ac2fc06d498b37 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.58ca3e60b9a645ba0a5d511fdcc729692035f66a596dc6f9b3573767e6b19181.42af86444c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T14:49:15.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">719ebf893cae98dddad268a10f4c837c </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.3e32a62d3c146ad838a365b3a46de69ad73ab6c5dd20b471d033c2fb24cb4905.fc02794631^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'] </t>
@@ -1319,13 +1319,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-10T13:50:58.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfab95ceb5dc473285ec1833de88f3c7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.b97cdf90132109cfc6c80299047a9017c829d411108f2ea0031737cd0e167a48.5a80e705d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T14:57:46.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">040a1ed1f53a60bef9e890e577e75e56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.88583aa707e6f165319fba695f8f3417b18af450d65cf21f8e27e989cadd3977.a82ac7adac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore di sintassi. ERROR: -1,-1 cvc-complex-type.2.4.b: The content of element 'order' is not complete. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id}' is expected. </t>
@@ -1338,13 +1338,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-10T15:08:25.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">c21fd35315abcf8471b70f84def20f54 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.921921c137a8fc65b182528e91b70190101abd6f6ba4973ad87fbb579e7e8611.b7f8205f3e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2026-02-24T15:01:48.000000Z </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c09640c9866f1ec5278e4a5d9da147ed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a0d43aed85b2c20a564071d064695678ed73f64017d9db84d73b55c397be6edc.02760cf2df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore di sintassi. ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":effectiveTime}'. One of '{\"urn:hl7-org:v3\":realmCode, \"urn:hl7-org:v3\":typeId, \"urn:hl7-org:v3\":templateId, \"urn:hl7-org:v3\":id, \"urn:hl7-org:v3\":code}' is expected.</t>
@@ -1357,13 +1357,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-11T09:56:48.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a613795733da25788096cf7f9695171d </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.7799df3193d1c86779f23c593be1b31d7acd8441a322bf8507f2e918ffc6f297.4cbad6b30e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T15:05:37.000000Z </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0dda249d77ad6d659153596206732862 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.872e13608bb1e975b9cb1809af476607ea0a6b7a6bb2151f6f1258101c31afb9.bfa1a6c8cf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-b4| Sezione Referto: la sezione DEVE essere presente],[ERRORE-b5| Sezione Referto: la sezione DEVE contenere un elemento 'text'] </t>
@@ -1376,13 +1376,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-11T11:04:29.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9eab6043663f2446a63e4e7a69dc661a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.7c6db5dd9aa3fbf05e0d65f9303f1c61867e2f95ec4c3a735df1c4a7a441580d.5eec9a816e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T15:10:51.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8cbcd3e779c17a65b2c937aa40342aec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.b22a7cff9ec67064d3b9667ad0f8d88868613ab24da22513f4265777524895a8.f4bb9eac9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-b6| Sezione Quesito Diagnostico: la sezione DEVE contenere un elemento 'text'] </t>
@@ -1395,13 +1395,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-16T09:44:23.000000Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75dda1016606895bbd0e57d4db6fb240</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.1e7e203c56bd295182cd7364ccd513a07373aa132e8824e0041a2edd3b56904b.3914f37836^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T15:15:35.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e501e376711647a7dd3e7a9f936ba667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.ac6aa1f9d43d74c1afdc1e1ca5cb2811af5be0fe6a90cfa18f182d7aefa0ec3a.c49a450b7e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-b3| Sezione Prestazioni: la sezione DEVE contenere un elemento 'entry']</t>
@@ -1414,13 +1414,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-16T11:41:23.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">d083cbfba9a5b9bef5e189ee5b263da2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.fd3d31333e3ba877fe21a5d6bb80eacb923adb91b26e047a302551d5005df668.812a92e875^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T15:49:11.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ffd448231edae29b38a81d3e07960e97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.66a60452980148c881e6184100764751370df91e91a1f7947ea5bd85d33d034b.b7c2c8fc2b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore Semantico. [ERRORE-b26| Sezione Storia Clinica: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato] </t>
@@ -1433,13 +1433,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-16T13:40:09.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">511341b0febde2d2709c65774eb9083c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.30307b1065cfdb413e558f23b40623aabcbd9852f3147ba0fd026c87c7c8f542.898f92d231^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T15:53:28.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">948570f4bf1089fa553601b678b9e26d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.580baed4036ff09cd18e111864a8f8be3e7c95845771a932a3cf0aae58820d42.0348b912f5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-b36| Sezione Storia Clinica: l'elemento entry/organizer/subject/relatedSubject deve avere l'attributo @classCode='PRS' e deve contenere l'elemento 'code'] </t>
@@ -1452,13 +1452,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 20" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-16T14:06:50.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">70b65c6f08b95005d127b2ec6503000e </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.2efa2adbf0fbc760a62d4bbff0ac32c8fa9b0c7a7342782c8f9b70a455c705f7.597c214a74^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T15:59:06.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b1d54abf6adff5cf0c6e765e7b7653cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.9f6eb3d38f56d4ff33a77b730361edaf0ce01d83b4e2ee9ac33d48171aff202e.513e28c7a6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-b53| Sotto-sezione Allergie: l'elemento entry/act/entryRelationship/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato ]</t>
@@ -1471,13 +1471,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-16T15:37:30.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">934db73ca733fd59a4c3595f6bc0740f </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.4af90d65b142fda056578d305c8738909fa6dafa0e3b7b3481ccdf7f8c9ea68d.d8678e9c2f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T16:05:27.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">502d993958387f5a103053d0a9f48ff3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.d625a85f9cbc769f9e6d754eb925c3f3c694de9312024e81e4a78e45cd3c3502.d326ad0d1a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-b57| Sotto-sezione Allergie: entry/act/entryRelationship/observation deve contenere almeno un elemento 'participant']</t>
@@ -1490,13 +1490,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 22" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-16T16:28:00.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a45162f8d415d4c725f1e1b46a7b1804 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.9391069a4bf2d4f280ef720ab3c207a2c7d7df69d4589346402e2771734b88b1.a6df52449e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T16:11:09.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ef2b88952cc9b5ad4f1a3bf5aca2a15e </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.4083b044cf08237b810817023fa5b230c3f25cd19a300df133f112e29b077d5d.5fa58fc2af^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 666.6] </t>
@@ -1509,13 +1509,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 23" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-17T10:45:05.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2ac3dd6ea990b44cb8dfbbd19a9668d7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.4f646b47dbbee1178fe83872e85c95c20fbac725bff71053194628b6c691ecda.d061b5b158^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T16:18:12.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52100084c66cb20d576ae47084eb4d49 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.81e6ae0882de355ffe4bd723680376bbdb52628987c8ae176f172e15c7f1eafe.f82f86f69d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore semantico. [ERRORE-30| L'elemento ClinicalDocument/legalAuthenticator/signatureCode deve essere valorizzato con il codice \"S\" ] </t>
@@ -1758,13 +1758,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-18T17:34:45.000000Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bf07a9b5f8f4093e1a0edb1371d9633e </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.4892d70ce75706dfe1a5ba06a8710a5d7581c0b09baf0a551fb009d8237d217f.298afb83d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T11:43:26.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8940b74d130d80bee35eef061dccd18f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.f472404fdf5b7d209387b6ddebb30f13132359332aaa634fb8de22287bd6e5e4.54cca43969^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_RSA_CT25</t>
@@ -1855,13 +1855,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 26" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-17T11:39:53.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">f8b548ba8a236cd3f9e3156ee71bec63 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.00b9ca115642264b61cbe4ae3429a07c5fc7bc3657ac87a1ba42d555b219527c.7a471e9ee1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T16:27:52.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1657d71d6bcd64f9db8cc11367006d32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.f4678a7a96b28cdb64a0f7a00043f97121f48148bce5c4a4c3750b5cd661e054.d34e6a09ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: 666.6]</t>
@@ -1928,13 +1928,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-17T14:51:18.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">69edbe38fc2566b572bda5f8fc1b7969</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a4c5c2a9b970270f441d5d91a414c870e2471a0387235ee91a42bb44b698e57f.91eccc46b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2026-02-24T16:31:28.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9c22889f01897c71998e7f37a15d3a1e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.081c37eb5b02318d2cdeb68f30a28b9ac5c6e9f7ba77e32e9566dbae54563cc7.8ae9e11c6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore di sintassi. ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{\"urn:hl7-org:v3\":languageCode}'. One of '{\"urn:hl7-org:v3\":confidentialityCode}' is expected. </t>
@@ -2004,13 +2004,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 28" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-02-17T15:01:43.000000Z </t>
-  </si>
-  <si>
-    <t xml:space="preserve">e85fadb9a77191e76dc830a1824fd9f3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a137364aee8404a5353a75b6ee3d88d9a08ee153e55bd8edbeed118597e990fb.4802a236ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2026-02-24T16:34:25.000000Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29c8a5d398d08eeb10a49ed089859816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.e940d3ac724ae2869cef1437b7cb729d5fe3c2ecc670afa0fb8a6711cc1b3aea.7dd26c09b8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore vocabolario. Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: X]</t>
@@ -2253,6 +2253,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2263,12 +2269,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2483,7 +2483,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2660,11 +2660,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2672,11 +2680,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3061,7 +3069,7 @@
   </sheetPr>
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3153,7 +3161,7 @@
   </sheetPr>
   <dimension ref="A1:B996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -4230,12 +4238,12 @@
   </sheetPr>
   <dimension ref="A1:W750"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D130" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="F130" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A130" activeCellId="0" sqref="A130"/>
-      <selection pane="bottomRight" activeCell="I164" activeCellId="0" sqref="I164"/>
+      <selection pane="bottomRight" activeCell="J190" activeCellId="0" sqref="J190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4744,7 +4752,7 @@
         <v>53</v>
       </c>
       <c r="F15" s="33" t="n">
-        <v>46062</v>
+        <v>46077</v>
       </c>
       <c r="G15" s="33" t="s">
         <v>69</v>
@@ -5084,7 +5092,7 @@
         <v>78</v>
       </c>
       <c r="F23" s="33" t="n">
-        <v>46062</v>
+        <v>46077</v>
       </c>
       <c r="G23" s="33" t="s">
         <v>86</v>
@@ -5426,7 +5434,7 @@
         <v>92</v>
       </c>
       <c r="F31" s="33" t="n">
-        <v>46062</v>
+        <v>46077</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="33"/>
@@ -8799,7 +8807,7 @@
         <v>291</v>
       </c>
       <c r="F117" s="33" t="n">
-        <v>46063</v>
+        <v>46077</v>
       </c>
       <c r="G117" s="42" t="s">
         <v>292</v>
@@ -8860,15 +8868,15 @@
         <v>297</v>
       </c>
       <c r="F118" s="33" t="n">
-        <v>46063</v>
-      </c>
-      <c r="G118" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G118" s="44" t="s">
         <v>298</v>
       </c>
-      <c r="H118" s="42" t="s">
+      <c r="H118" s="44" t="s">
         <v>299</v>
       </c>
-      <c r="I118" s="39" t="s">
+      <c r="I118" s="43" t="s">
         <v>300</v>
       </c>
       <c r="J118" s="34" t="s">
@@ -8882,7 +8890,7 @@
       <c r="N118" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O118" s="44" t="s">
+      <c r="O118" s="45" t="s">
         <v>301</v>
       </c>
       <c r="P118" s="34" t="s">
@@ -8962,12 +8970,12 @@
         <v>305</v>
       </c>
       <c r="F120" s="33" t="n">
-        <v>46063</v>
-      </c>
-      <c r="G120" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G120" s="44" t="s">
         <v>306</v>
       </c>
-      <c r="H120" s="42" t="s">
+      <c r="H120" s="44" t="s">
         <v>307</v>
       </c>
       <c r="I120" s="39" t="s">
@@ -9023,7 +9031,7 @@
         <v>311</v>
       </c>
       <c r="F121" s="33" t="n">
-        <v>46063</v>
+        <v>46077</v>
       </c>
       <c r="G121" s="42" t="s">
         <v>312</v>
@@ -9045,7 +9053,7 @@
       <c r="N121" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O121" s="44" t="s">
+      <c r="O121" s="45" t="s">
         <v>315</v>
       </c>
       <c r="P121" s="34" t="s">
@@ -9084,7 +9092,7 @@
         <v>317</v>
       </c>
       <c r="F122" s="33" t="n">
-        <v>46064</v>
+        <v>46077</v>
       </c>
       <c r="G122" s="39" t="s">
         <v>318</v>
@@ -9106,7 +9114,7 @@
       <c r="N122" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O122" s="44" t="s">
+      <c r="O122" s="45" t="s">
         <v>321</v>
       </c>
       <c r="P122" s="34" t="s">
@@ -9145,12 +9153,12 @@
         <v>323</v>
       </c>
       <c r="F123" s="33" t="n">
-        <v>46064</v>
-      </c>
-      <c r="G123" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G123" s="44" t="s">
         <v>324</v>
       </c>
-      <c r="H123" s="42" t="s">
+      <c r="H123" s="44" t="s">
         <v>325</v>
       </c>
       <c r="I123" s="39" t="s">
@@ -9167,7 +9175,7 @@
       <c r="N123" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O123" s="44" t="s">
+      <c r="O123" s="45" t="s">
         <v>327</v>
       </c>
       <c r="P123" s="34" t="s">
@@ -9206,9 +9214,9 @@
         <v>329</v>
       </c>
       <c r="F124" s="33" t="n">
-        <v>46069</v>
-      </c>
-      <c r="G124" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G124" s="44" t="s">
         <v>330</v>
       </c>
       <c r="H124" s="39" t="s">
@@ -9228,7 +9236,7 @@
       <c r="N124" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O124" s="44" t="s">
+      <c r="O124" s="45" t="s">
         <v>333</v>
       </c>
       <c r="P124" s="34" t="s">
@@ -9267,12 +9275,12 @@
         <v>335</v>
       </c>
       <c r="F125" s="33" t="n">
-        <v>46069</v>
-      </c>
-      <c r="G125" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G125" s="44" t="s">
         <v>336</v>
       </c>
-      <c r="H125" s="42" t="s">
+      <c r="H125" s="44" t="s">
         <v>337</v>
       </c>
       <c r="I125" s="39" t="s">
@@ -9289,7 +9297,7 @@
       <c r="N125" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O125" s="44" t="s">
+      <c r="O125" s="45" t="s">
         <v>339</v>
       </c>
       <c r="P125" s="34" t="s">
@@ -9328,15 +9336,15 @@
         <v>341</v>
       </c>
       <c r="F126" s="33" t="n">
-        <v>46069</v>
-      </c>
-      <c r="G126" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G126" s="44" t="s">
         <v>342</v>
       </c>
-      <c r="H126" s="42" t="s">
+      <c r="H126" s="44" t="s">
         <v>343</v>
       </c>
-      <c r="I126" s="43" t="s">
+      <c r="I126" s="46" t="s">
         <v>344</v>
       </c>
       <c r="J126" s="34" t="s">
@@ -9350,7 +9358,7 @@
       <c r="N126" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O126" s="44" t="s">
+      <c r="O126" s="45" t="s">
         <v>345</v>
       </c>
       <c r="P126" s="34" t="s">
@@ -9389,15 +9397,15 @@
         <v>347</v>
       </c>
       <c r="F127" s="33" t="n">
-        <v>46069</v>
-      </c>
-      <c r="G127" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G127" s="44" t="s">
         <v>348</v>
       </c>
-      <c r="H127" s="42" t="s">
+      <c r="H127" s="44" t="s">
         <v>349</v>
       </c>
-      <c r="I127" s="43" t="s">
+      <c r="I127" s="46" t="s">
         <v>350</v>
       </c>
       <c r="J127" s="34" t="s">
@@ -9450,15 +9458,15 @@
         <v>353</v>
       </c>
       <c r="F128" s="33" t="n">
-        <v>46069</v>
-      </c>
-      <c r="G128" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G128" s="44" t="s">
         <v>354</v>
       </c>
-      <c r="H128" s="42" t="s">
+      <c r="H128" s="44" t="s">
         <v>355</v>
       </c>
-      <c r="I128" s="43" t="s">
+      <c r="I128" s="46" t="s">
         <v>356</v>
       </c>
       <c r="J128" s="34" t="s">
@@ -9511,15 +9519,15 @@
         <v>359</v>
       </c>
       <c r="F129" s="33" t="n">
-        <v>46069</v>
-      </c>
-      <c r="G129" s="42" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G129" s="44" t="s">
         <v>360</v>
       </c>
-      <c r="H129" s="42" t="s">
+      <c r="H129" s="44" t="s">
         <v>361</v>
       </c>
-      <c r="I129" s="43" t="s">
+      <c r="I129" s="46" t="s">
         <v>362</v>
       </c>
       <c r="J129" s="34" t="s">
@@ -9572,12 +9580,12 @@
         <v>365</v>
       </c>
       <c r="F130" s="33" t="n">
-        <v>46070</v>
-      </c>
-      <c r="G130" s="45" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G130" s="47" t="s">
         <v>366</v>
       </c>
-      <c r="H130" s="45" t="s">
+      <c r="H130" s="47" t="s">
         <v>367</v>
       </c>
       <c r="I130" s="39" t="s">
@@ -9594,7 +9602,7 @@
       <c r="N130" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="O130" s="44" t="s">
+      <c r="O130" s="45" t="s">
         <v>369</v>
       </c>
       <c r="P130" s="34" t="s">
@@ -10844,7 +10852,7 @@
       <c r="B164" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C164" s="46" t="s">
+      <c r="C164" s="48" t="s">
         <v>67</v>
       </c>
       <c r="D164" s="30" t="s">
@@ -10854,7 +10862,7 @@
         <v>436</v>
       </c>
       <c r="F164" s="33" t="n">
-        <v>46071</v>
+        <v>46077</v>
       </c>
       <c r="G164" s="47" t="s">
         <v>437</v>
@@ -10862,7 +10870,7 @@
       <c r="H164" s="47" t="s">
         <v>438</v>
       </c>
-      <c r="I164" s="39" t="s">
+      <c r="I164" s="49" t="s">
         <v>439</v>
       </c>
       <c r="J164" s="34" t="s">
@@ -10900,9 +10908,7 @@
       <c r="E165" s="31" t="s">
         <v>441</v>
       </c>
-      <c r="F165" s="33" t="n">
-        <v>46071</v>
-      </c>
+      <c r="F165" s="33"/>
       <c r="G165" s="33"/>
       <c r="H165" s="33"/>
       <c r="I165" s="39"/>
@@ -11314,9 +11320,9 @@
         <v>464</v>
       </c>
       <c r="F176" s="33" t="n">
-        <v>46070</v>
-      </c>
-      <c r="G176" s="48" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G176" s="50" t="s">
         <v>465</v>
       </c>
       <c r="H176" s="33" t="s">
@@ -11621,15 +11627,15 @@
         <v>486</v>
       </c>
       <c r="F183" s="33" t="n">
-        <v>46070</v>
-      </c>
-      <c r="G183" s="48" t="s">
+        <v>46077</v>
+      </c>
+      <c r="G183" s="50" t="s">
         <v>487</v>
       </c>
-      <c r="H183" s="42" t="s">
+      <c r="H183" s="44" t="s">
         <v>488</v>
       </c>
-      <c r="I183" s="43" t="s">
+      <c r="I183" s="46" t="s">
         <v>489</v>
       </c>
       <c r="J183" s="34" t="s">
@@ -11746,7 +11752,7 @@
       <c r="B186" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C186" s="49" t="s">
+      <c r="C186" s="51" t="s">
         <v>59</v>
       </c>
       <c r="D186" s="30" t="s">
@@ -11924,7 +11930,7 @@
         <v>509</v>
       </c>
       <c r="F190" s="33" t="n">
-        <v>46070</v>
+        <v>46077</v>
       </c>
       <c r="G190" s="33" t="s">
         <v>510</v>
@@ -12055,7 +12061,7 @@
       <c r="D193" s="30" t="s">
         <v>518</v>
       </c>
-      <c r="E193" s="50" t="s">
+      <c r="E193" s="52" t="s">
         <v>519</v>
       </c>
       <c r="F193" s="33"/>
@@ -16090,7 +16096,7 @@
   </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -16154,7 +16160,7 @@
   </sheetPr>
   <dimension ref="A1:G960"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
@@ -16172,7 +16178,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>523</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -16184,158 +16190,158 @@
       <c r="D1" s="19" t="s">
         <v>525</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="54" t="s">
         <v>526</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="55" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="57" t="s">
         <v>529</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="58" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="57" t="s">
         <v>531</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="58" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="57" t="s">
         <v>533</v>
       </c>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="59" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="57" t="s">
         <v>535</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="58" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="57" t="s">
         <v>537</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="59" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="57" t="s">
         <v>539</v>
       </c>
-      <c r="D7" s="57" t="s">
+      <c r="D7" s="59" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="57" t="s">
         <v>541</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="59" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="57" t="s">
         <v>543</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="59" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="36.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="56" t="s">
         <v>545</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="60" t="s">
         <v>546</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="58" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="56" t="s">
         <v>404</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="57" t="s">
         <v>548</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="59" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D12" s="59"/>
+      <c r="D12" s="61"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D13" s="59"/>
+      <c r="D13" s="61"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -17304,7 +17310,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -17316,32 +17322,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="62" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="62" t="s">
         <v>550</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="62" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="62" t="s">
         <v>551</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="62" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>